<commit_message>
Change time between judging sessions
</commit_message>
<xml_diff>
--- a/scheduler/schedule.xlsx
+++ b/scheduler/schedule.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>OFFICIAL ROBOT ROUNDS SCHEDULE</t>
   </si>
@@ -131,9 +131,6 @@
   </si>
   <si>
     <t>12:52-1:00</t>
-  </si>
-  <si>
-    <t>1:00-1:08</t>
   </si>
 </sst>
 </file>
@@ -497,7 +494,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -657,22 +654,22 @@
         <v>13</v>
       </c>
       <c r="C7" s="3">
-        <v>12008</v>
+        <v>12014</v>
       </c>
       <c r="D7" s="3">
-        <v>12010</v>
+        <v>12016</v>
       </c>
       <c r="E7" s="3">
-        <v>12011</v>
+        <v>12013</v>
       </c>
       <c r="F7" s="3">
-        <v>12013</v>
+        <v>12015</v>
       </c>
       <c r="G7" s="3">
-        <v>12012</v>
+        <v>12019</v>
       </c>
       <c r="H7" s="3">
-        <v>12014</v>
+        <v>12017</v>
       </c>
     </row>
     <row r="8" spans="1:8">
@@ -683,22 +680,22 @@
         <v>14</v>
       </c>
       <c r="C8" s="3">
-        <v>12015</v>
+        <v>12020</v>
       </c>
       <c r="D8" s="3">
-        <v>12017</v>
+        <v>12018</v>
       </c>
       <c r="E8" s="3">
-        <v>12016</v>
+        <v>12022</v>
       </c>
       <c r="F8" s="3">
-        <v>12018</v>
+        <v>12024</v>
       </c>
       <c r="G8" s="3">
-        <v>12019</v>
+        <v>12021</v>
       </c>
       <c r="H8" s="3">
-        <v>12021</v>
+        <v>12023</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -763,22 +760,22 @@
         <v>18</v>
       </c>
       <c r="C12" s="3">
-        <v>12020</v>
+        <v>12016</v>
       </c>
       <c r="D12" s="3">
-        <v>12022</v>
+        <v>12013</v>
       </c>
       <c r="E12" s="3">
-        <v>12023</v>
+        <v>12026</v>
       </c>
       <c r="F12" s="3">
+        <v>12028</v>
+      </c>
+      <c r="G12" s="3">
         <v>12025</v>
       </c>
-      <c r="G12" s="3">
-        <v>12024</v>
-      </c>
       <c r="H12" s="3">
-        <v>12026</v>
+        <v>12027</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -789,22 +786,22 @@
         <v>19</v>
       </c>
       <c r="C13" s="3">
-        <v>12014</v>
+        <v>12021</v>
       </c>
       <c r="D13" s="3">
-        <v>12028</v>
+        <v>12019</v>
       </c>
       <c r="E13" s="3">
-        <v>12013</v>
+        <v>12001</v>
       </c>
       <c r="F13" s="3">
-        <v>12027</v>
+        <v>12023</v>
       </c>
       <c r="G13" s="3">
-        <v>12018</v>
+        <v>12020</v>
       </c>
       <c r="H13" s="3">
-        <v>12015</v>
+        <v>12022</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -818,19 +815,19 @@
         <v>12002</v>
       </c>
       <c r="D14" s="3">
-        <v>12021</v>
+        <v>12024</v>
       </c>
       <c r="E14" s="3">
-        <v>12001</v>
+        <v>12004</v>
       </c>
       <c r="F14" s="3">
-        <v>12019</v>
+        <v>12006</v>
       </c>
       <c r="G14" s="3">
-        <v>12016</v>
+        <v>12003</v>
       </c>
       <c r="H14" s="3">
-        <v>12017</v>
+        <v>12005</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -841,22 +838,22 @@
         <v>21</v>
       </c>
       <c r="C15" s="3">
-        <v>12003</v>
+        <v>12008</v>
       </c>
       <c r="D15" s="3">
-        <v>12005</v>
+        <v>12010</v>
       </c>
       <c r="E15" s="3">
-        <v>12004</v>
+        <v>12007</v>
       </c>
       <c r="F15" s="3">
-        <v>12006</v>
+        <v>12011</v>
       </c>
       <c r="G15" s="3">
-        <v>12020</v>
+        <v>12012</v>
       </c>
       <c r="H15" s="3">
-        <v>12023</v>
+        <v>12009</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -867,22 +864,22 @@
         <v>22</v>
       </c>
       <c r="C16" s="3">
-        <v>12022</v>
+        <v>12026</v>
       </c>
       <c r="D16" s="3">
-        <v>12024</v>
+        <v>12027</v>
       </c>
       <c r="E16" s="3">
-        <v>12026</v>
+        <v>12019</v>
       </c>
       <c r="F16" s="3">
+        <v>12001</v>
+      </c>
+      <c r="G16" s="3">
         <v>12028</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>12025</v>
-      </c>
-      <c r="H16" s="3">
-        <v>12027</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -921,22 +918,22 @@
         <v>25</v>
       </c>
       <c r="C19" s="3">
-        <v>12011</v>
+        <v>12004</v>
       </c>
       <c r="D19" s="3">
-        <v>12001</v>
+        <v>12005</v>
       </c>
       <c r="E19" s="3">
-        <v>12008</v>
+        <v>12002</v>
       </c>
       <c r="F19" s="3">
-        <v>12009</v>
+        <v>12003</v>
       </c>
       <c r="G19" s="3">
+        <v>12006</v>
+      </c>
+      <c r="H19" s="3">
         <v>12007</v>
-      </c>
-      <c r="H19" s="3">
-        <v>12010</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -947,22 +944,22 @@
         <v>26</v>
       </c>
       <c r="C20" s="3">
-        <v>12021</v>
+        <v>12012</v>
       </c>
       <c r="D20" s="3">
-        <v>12004</v>
+        <v>12001</v>
       </c>
       <c r="E20" s="3">
-        <v>12002</v>
+        <v>12008</v>
       </c>
       <c r="F20" s="3">
-        <v>12012</v>
+        <v>12009</v>
       </c>
       <c r="G20" s="3">
-        <v>12003</v>
+        <v>12010</v>
       </c>
       <c r="H20" s="3">
-        <v>12019</v>
+        <v>12011</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -973,22 +970,22 @@
         <v>27</v>
       </c>
       <c r="C21" s="3">
-        <v>12006</v>
+        <v>12013</v>
       </c>
       <c r="D21" s="3">
-        <v>12023</v>
+        <v>12017</v>
       </c>
       <c r="E21" s="3">
-        <v>12005</v>
+        <v>12016</v>
       </c>
       <c r="F21" s="3">
-        <v>12020</v>
+        <v>12018</v>
       </c>
       <c r="G21" s="3">
-        <v>12022</v>
+        <v>12014</v>
       </c>
       <c r="H21" s="3">
-        <v>12025</v>
+        <v>12015</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -999,22 +996,22 @@
         <v>28</v>
       </c>
       <c r="C22" s="3">
-        <v>12024</v>
+        <v>12027</v>
       </c>
       <c r="D22" s="3">
-        <v>12027</v>
+        <v>12004</v>
       </c>
       <c r="E22" s="3">
-        <v>12028</v>
+        <v>12002</v>
       </c>
       <c r="F22" s="3">
-        <v>12007</v>
+        <v>12025</v>
       </c>
       <c r="G22" s="3">
         <v>12026</v>
       </c>
       <c r="H22" s="3">
-        <v>12001</v>
+        <v>12003</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -1025,22 +1022,22 @@
         <v>29</v>
       </c>
       <c r="C23" s="3">
-        <v>12002</v>
+        <v>12001</v>
       </c>
       <c r="D23" s="3">
-        <v>12009</v>
+        <v>12006</v>
       </c>
       <c r="E23" s="3">
+        <v>12028</v>
+      </c>
+      <c r="F23" s="3">
+        <v>12005</v>
+      </c>
+      <c r="G23" s="3">
+        <v>12007</v>
+      </c>
+      <c r="H23" s="3">
         <v>12010</v>
-      </c>
-      <c r="F23" s="3">
-        <v>12003</v>
-      </c>
-      <c r="G23" s="3">
-        <v>12008</v>
-      </c>
-      <c r="H23" s="3">
-        <v>12011</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1051,22 +1048,22 @@
         <v>30</v>
       </c>
       <c r="C24" s="3">
-        <v>12004</v>
+        <v>12008</v>
       </c>
       <c r="D24" s="3">
+        <v>12011</v>
+      </c>
+      <c r="E24" s="3">
         <v>12012</v>
       </c>
-      <c r="E24" s="3">
-        <v>12006</v>
-      </c>
       <c r="F24" s="3">
-        <v>12001</v>
+        <v>12014</v>
       </c>
       <c r="G24" s="3">
-        <v>12025</v>
+        <v>12009</v>
       </c>
       <c r="H24" s="3">
-        <v>12005</v>
+        <v>12013</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1105,22 +1102,22 @@
         <v>33</v>
       </c>
       <c r="C27" s="3">
-        <v>12007</v>
+        <v>12022</v>
       </c>
       <c r="D27" s="3">
-        <v>12016</v>
+        <v>12023</v>
       </c>
       <c r="E27" s="3">
-        <v>12018</v>
+        <v>12020</v>
       </c>
       <c r="F27" s="3">
-        <v>12014</v>
+        <v>12021</v>
       </c>
       <c r="G27" s="3">
-        <v>12015</v>
+        <v>12024</v>
       </c>
       <c r="H27" s="3">
-        <v>12013</v>
+        <v>12019</v>
       </c>
     </row>
     <row r="28" spans="1:8">
@@ -1134,19 +1131,19 @@
         <v>12017</v>
       </c>
       <c r="D28" s="3">
-        <v>12026</v>
+        <v>12015</v>
       </c>
       <c r="E28" s="3">
-        <v>12027</v>
+        <v>12018</v>
       </c>
       <c r="F28" s="3">
+        <v>12003</v>
+      </c>
+      <c r="G28" s="3">
         <v>12002</v>
       </c>
-      <c r="G28" s="3">
-        <v>12028</v>
-      </c>
       <c r="H28" s="3">
-        <v>12003</v>
+        <v>12016</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1157,22 +1154,22 @@
         <v>35</v>
       </c>
       <c r="C29" s="3">
+        <v>12006</v>
+      </c>
+      <c r="D29" s="3">
+        <v>12011</v>
+      </c>
+      <c r="E29" s="3">
         <v>12005</v>
       </c>
-      <c r="D29" s="3">
-        <v>12010</v>
-      </c>
-      <c r="E29" s="3">
-        <v>12009</v>
-      </c>
       <c r="F29" s="3">
-        <v>12011</v>
+        <v>12008</v>
       </c>
       <c r="G29" s="3">
         <v>12004</v>
       </c>
       <c r="H29" s="3">
-        <v>12008</v>
+        <v>12010</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1183,22 +1180,22 @@
         <v>36</v>
       </c>
       <c r="C30" s="3">
+        <v>12015</v>
+      </c>
+      <c r="D30" s="3">
+        <v>12022</v>
+      </c>
+      <c r="E30" s="3">
         <v>12012</v>
       </c>
-      <c r="D30" s="3">
-        <v>12006</v>
-      </c>
-      <c r="E30" s="3">
+      <c r="F30" s="3">
+        <v>12020</v>
+      </c>
+      <c r="G30" s="3">
         <v>12014</v>
       </c>
-      <c r="F30" s="3">
-        <v>12015</v>
-      </c>
-      <c r="G30" s="3">
-        <v>12013</v>
-      </c>
       <c r="H30" s="3">
-        <v>12016</v>
+        <v>12021</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -1211,13 +1208,17 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3">
+        <v>12023</v>
+      </c>
+      <c r="F31" s="3">
         <v>12017</v>
       </c>
-      <c r="F31" s="3">
+      <c r="G31" s="3">
         <v>12018</v>
       </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
+      <c r="H31" s="3">
+        <v>12024</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="3">
@@ -1226,38 +1227,20 @@
       <c r="B32" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="C32" s="3">
+        <v>12025</v>
+      </c>
+      <c r="D32" s="3">
+        <v>12026</v>
+      </c>
+      <c r="E32" s="3">
+        <v>12027</v>
+      </c>
+      <c r="F32" s="3">
+        <v>12028</v>
+      </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-    </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="3">
-        <v>31</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C33" s="3">
-        <v>12022</v>
-      </c>
-      <c r="D33" s="3">
-        <v>12019</v>
-      </c>
-      <c r="E33" s="3">
-        <v>12024</v>
-      </c>
-      <c r="F33" s="3">
-        <v>12023</v>
-      </c>
-      <c r="G33" s="3">
-        <v>12021</v>
-      </c>
-      <c r="H33" s="3">
-        <v>12020</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Remove zero padding from hour
</commit_message>
<xml_diff>
--- a/scheduler/schedule.xlsx
+++ b/scheduler/schedule.xlsx
@@ -47,49 +47,49 @@
     <t>Blue 2</t>
   </si>
   <si>
-    <t>02:00-02:08</t>
-  </si>
-  <si>
-    <t>02:08-02:16</t>
-  </si>
-  <si>
-    <t>02:16-02:24</t>
-  </si>
-  <si>
-    <t>02:24-02:32</t>
-  </si>
-  <si>
-    <t>02:32-02:40</t>
-  </si>
-  <si>
-    <t>02:40-02:48</t>
-  </si>
-  <si>
-    <t>02:48-02:56</t>
-  </si>
-  <si>
-    <t>02:56-03:04</t>
-  </si>
-  <si>
-    <t>03:04-03:12</t>
-  </si>
-  <si>
-    <t>03:12-03:20</t>
-  </si>
-  <si>
-    <t>03:20-03:28</t>
-  </si>
-  <si>
-    <t>03:28-03:36</t>
-  </si>
-  <si>
-    <t>03:36-03:44</t>
-  </si>
-  <si>
-    <t>03:44-03:52</t>
-  </si>
-  <si>
-    <t>03:52-04:00</t>
+    <t>2:00-2:08</t>
+  </si>
+  <si>
+    <t>2:08-2:16</t>
+  </si>
+  <si>
+    <t>2:16-2:24</t>
+  </si>
+  <si>
+    <t>2:24-2:32</t>
+  </si>
+  <si>
+    <t>2:32-2:40</t>
+  </si>
+  <si>
+    <t>2:40-2:48</t>
+  </si>
+  <si>
+    <t>2:48-2:56</t>
+  </si>
+  <si>
+    <t>2:56-3:04</t>
+  </si>
+  <si>
+    <t>3:04-3:12</t>
+  </si>
+  <si>
+    <t>3:12-3:20</t>
+  </si>
+  <si>
+    <t>3:20-3:28</t>
+  </si>
+  <si>
+    <t>3:28-3:36</t>
+  </si>
+  <si>
+    <t>3:36-3:44</t>
+  </si>
+  <si>
+    <t>3:44-3:52</t>
+  </si>
+  <si>
+    <t>3:52-4:00</t>
   </si>
   <si>
     <t>JUDGING SESSION SCHEDULE</t>
@@ -98,31 +98,31 @@
     <t>Room 108</t>
   </si>
   <si>
-    <t>02:00-02:10</t>
-  </si>
-  <si>
-    <t>02:15-02:25</t>
-  </si>
-  <si>
-    <t>02:30-02:40</t>
-  </si>
-  <si>
-    <t>02:45-02:55</t>
-  </si>
-  <si>
-    <t>03:00-03:10</t>
-  </si>
-  <si>
-    <t>03:15-03:25</t>
-  </si>
-  <si>
-    <t>03:30-03:40</t>
-  </si>
-  <si>
-    <t>03:45-03:55</t>
-  </si>
-  <si>
-    <t>04:00-04:10</t>
+    <t>2:00-2:10</t>
+  </si>
+  <si>
+    <t>2:15-2:25</t>
+  </si>
+  <si>
+    <t>2:30-2:40</t>
+  </si>
+  <si>
+    <t>2:45-2:55</t>
+  </si>
+  <si>
+    <t>3:00-3:10</t>
+  </si>
+  <si>
+    <t>3:15-3:25</t>
+  </si>
+  <si>
+    <t>3:30-3:40</t>
+  </si>
+  <si>
+    <t>3:45-3:55</t>
+  </si>
+  <si>
+    <t>4:00-4:10</t>
   </si>
   <si>
     <t>TEAM 12001 SCHEDULE</t>

</xml_diff>

<commit_message>
Add creation of "All Matches" sheet for printing Manually merged from Aryan branch
</commit_message>
<xml_diff>
--- a/scheduler/schedule.xlsx
+++ b/scheduler/schedule.xlsx
@@ -9,15 +9,16 @@
   <sheets>
     <sheet name="Match Schedule" sheetId="1" r:id="rId1"/>
     <sheet name="Judging Schedule" sheetId="2" r:id="rId2"/>
-    <sheet name="Team 12001 Schedule" sheetId="3" r:id="rId3"/>
-    <sheet name="Team 12002 Schedule" sheetId="4" r:id="rId4"/>
-    <sheet name="Team 12003 Schedule" sheetId="5" r:id="rId5"/>
-    <sheet name="Team 12004 Schedule" sheetId="6" r:id="rId6"/>
-    <sheet name="Team 12005 Schedule" sheetId="7" r:id="rId7"/>
-    <sheet name="Team 12006 Schedule" sheetId="8" r:id="rId8"/>
-    <sheet name="Team 12007 Schedule" sheetId="9" r:id="rId9"/>
-    <sheet name="Team 12008 Schedule" sheetId="10" r:id="rId10"/>
-    <sheet name="Team 12009 Schedule" sheetId="11" r:id="rId11"/>
+    <sheet name="All Matches" sheetId="3" r:id="rId3"/>
+    <sheet name="Team 12001 Schedule" sheetId="4" r:id="rId4"/>
+    <sheet name="Team 12002 Schedule" sheetId="5" r:id="rId5"/>
+    <sheet name="Team 12003 Schedule" sheetId="6" r:id="rId6"/>
+    <sheet name="Team 12004 Schedule" sheetId="7" r:id="rId7"/>
+    <sheet name="Team 12005 Schedule" sheetId="8" r:id="rId8"/>
+    <sheet name="Team 12006 Schedule" sheetId="9" r:id="rId9"/>
+    <sheet name="Team 12007 Schedule" sheetId="10" r:id="rId10"/>
+    <sheet name="Team 12008 Schedule" sheetId="11" r:id="rId11"/>
+    <sheet name="Team 12009 Schedule" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -936,7 +937,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -960,7 +961,7 @@
         <v>59</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -971,15 +972,15 @@
         <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>45</v>
@@ -987,35 +988,35 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1027,6 +1028,109 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -1237,103 +1341,508 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="18.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="A1">
+        <v>12001</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
+      <c r="A2">
+        <v>12001</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
+      <c r="A3">
+        <v>12001</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="A4">
+        <v>12001</v>
+      </c>
+      <c r="B4">
         <v>10</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>38</v>
+      <c r="C4">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="A5">
+        <v>12001</v>
+      </c>
+      <c r="B5">
         <v>12</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
+      <c r="C5">
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="A6">
+        <v>12002</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>12002</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>12002</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>12002</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>12002</v>
+      </c>
+      <c r="B10">
         <v>14</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>45</v>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>12003</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>12003</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12003</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>12003</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>12003</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>12004</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>12004</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>12004</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>12004</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>12004</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>12005</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>12005</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>12005</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>12005</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>12005</v>
+      </c>
+      <c r="B25">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>12006</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>12006</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>12006</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>12006</v>
+      </c>
+      <c r="B29">
+        <v>7</v>
+      </c>
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>12006</v>
+      </c>
+      <c r="B30">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>12007</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>12007</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>12007</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>12007</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>12007</v>
+      </c>
+      <c r="B35">
+        <v>15</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>12008</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>12008</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>12008</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>12008</v>
+      </c>
+      <c r="B39">
+        <v>9</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>12008</v>
+      </c>
+      <c r="B40">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>12009</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>12009</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>12009</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>12009</v>
+      </c>
+      <c r="B44">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>12009</v>
+      </c>
+      <c r="B45">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1351,7 +1860,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1369,7 +1878,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>36</v>
@@ -1380,10 +1889,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>38</v>
@@ -1391,10 +1900,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>40</v>
@@ -1402,35 +1911,35 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1454,7 +1963,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1472,24 +1981,24 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1500,7 +2009,7 @@
         <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1511,7 +2020,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1522,7 +2031,7 @@
         <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1533,7 +2042,7 @@
         <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1557,7 +2066,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1581,29 +2090,29 @@
         <v>49</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1614,7 +2123,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1625,7 +2134,7 @@
         <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1636,7 +2145,7 @@
         <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1660,7 +2169,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1684,7 +2193,7 @@
         <v>49</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1695,37 +2204,37 @@
         <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>38</v>
@@ -1733,13 +2242,13 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1763,7 +2272,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1787,7 +2296,7 @@
         <v>49</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1798,7 +2307,7 @@
         <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1809,29 +2318,29 @@
         <v>53</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1842,7 +2351,7 @@
         <v>55</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1866,7 +2375,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1884,21 +2393,21 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>40</v>
@@ -1906,29 +2415,29 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>36</v>
@@ -1939,10 +2448,10 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
Add schedule for each table
</commit_message>
<xml_diff>
--- a/scheduler/schedule.xlsx
+++ b/scheduler/schedule.xlsx
@@ -9,23 +9,27 @@
   <sheets>
     <sheet name="Match Schedule" sheetId="1" r:id="rId1"/>
     <sheet name="Judging Schedule" sheetId="2" r:id="rId2"/>
-    <sheet name="All Matches" sheetId="3" r:id="rId3"/>
-    <sheet name="Team 12001 Schedule" sheetId="4" r:id="rId4"/>
-    <sheet name="Team 12002 Schedule" sheetId="5" r:id="rId5"/>
-    <sheet name="Team 12003 Schedule" sheetId="6" r:id="rId6"/>
-    <sheet name="Team 12004 Schedule" sheetId="7" r:id="rId7"/>
-    <sheet name="Team 12005 Schedule" sheetId="8" r:id="rId8"/>
-    <sheet name="Team 12006 Schedule" sheetId="9" r:id="rId9"/>
-    <sheet name="Team 12007 Schedule" sheetId="10" r:id="rId10"/>
-    <sheet name="Team 12008 Schedule" sheetId="11" r:id="rId11"/>
-    <sheet name="Team 12009 Schedule" sheetId="12" r:id="rId12"/>
+    <sheet name="Table R1 Schedule" sheetId="3" r:id="rId3"/>
+    <sheet name="Table R2 Schedule" sheetId="4" r:id="rId4"/>
+    <sheet name="Table B1 Schedule" sheetId="5" r:id="rId5"/>
+    <sheet name="Table B2 Schedule" sheetId="6" r:id="rId6"/>
+    <sheet name="All Matches" sheetId="7" r:id="rId7"/>
+    <sheet name="Team 12001 Schedule" sheetId="8" r:id="rId8"/>
+    <sheet name="Team 12002 Schedule" sheetId="9" r:id="rId9"/>
+    <sheet name="Team 12003 Schedule" sheetId="10" r:id="rId10"/>
+    <sheet name="Team 12004 Schedule" sheetId="11" r:id="rId11"/>
+    <sheet name="Team 12005 Schedule" sheetId="12" r:id="rId12"/>
+    <sheet name="Team 12006 Schedule" sheetId="13" r:id="rId13"/>
+    <sheet name="Team 12007 Schedule" sheetId="14" r:id="rId14"/>
+    <sheet name="Team 12008 Schedule" sheetId="15" r:id="rId15"/>
+    <sheet name="Team 12009 Schedule" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="69">
   <si>
     <t>OFFICIAL ROBOT ROUNDS SCHEDULE</t>
   </si>
@@ -124,6 +128,21 @@
   </si>
   <si>
     <t>4:00-4:10</t>
+  </si>
+  <si>
+    <t>TABLE R1 SCHEDULE</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>TABLE R2 SCHEDULE</t>
+  </si>
+  <si>
+    <t>TABLE B1 SCHEDULE</t>
+  </si>
+  <si>
+    <t>TABLE B2 SCHEDULE</t>
   </si>
   <si>
     <t>TEAM 12001 SCHEDULE</t>
@@ -240,7 +259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +275,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -312,6 +337,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -936,84 +962,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="A1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>45</v>
@@ -1039,29 +1065,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="A1" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>45</v>
@@ -1069,57 +1095,57 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1142,21 +1168,227 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="A1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1164,10 +1396,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1175,7 +1407,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>45</v>
@@ -1186,10 +1418,113 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="C5" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1197,10 +1532,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1208,10 +1543,113 @@
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1219,7 +1657,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>23</v>
@@ -1341,6 +1779,498 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>12003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3">
+        <v>12002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3">
+        <v>12007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3">
+        <v>12004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3">
+        <v>12005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3">
+        <v>12004</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>12004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>12007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>12005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3">
+        <v>12002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="3">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="3">
+        <v>12003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3">
+        <v>12003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>12005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>12007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>12004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3">
+        <v>12003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="3">
+        <v>12002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3">
+        <v>12005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3">
+        <v>12002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="3">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3">
+        <v>12005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3">
+        <v>12007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3">
+        <v>12003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3">
+        <v>12002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="3">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="3">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="3">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="3">
+        <v>12004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="3">
+        <v>12007</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1843,418 +2773,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="18.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="18.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="18.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="18.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2271,87 +2789,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="A1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2374,87 +2892,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="A1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add option to avoid leaving teams without an opponent
</commit_message>
<xml_diff>
--- a/scheduler/schedule.xlsx
+++ b/scheduler/schedule.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="70">
   <si>
     <t>OFFICIAL ROBOT ROUNDS SCHEDULE</t>
   </si>
@@ -97,6 +97,9 @@
     <t>3:52-4:00</t>
   </si>
   <si>
+    <t>4:00-4:08</t>
+  </si>
+  <si>
     <t>JUDGING SESSION SCHEDULE</t>
   </si>
   <si>
@@ -160,34 +163,43 @@
     <t>Match 4</t>
   </si>
   <si>
+    <t>Table B1</t>
+  </si>
+  <si>
+    <t>Match 6</t>
+  </si>
+  <si>
+    <t>Table B2</t>
+  </si>
+  <si>
+    <t>Match 8</t>
+  </si>
+  <si>
     <t>Table R1</t>
   </si>
   <si>
-    <t>Match 6</t>
+    <t>Match 10</t>
+  </si>
+  <si>
+    <t>Match 12</t>
   </si>
   <si>
     <t>Table R2</t>
   </si>
   <si>
-    <t>Match 8</t>
-  </si>
-  <si>
-    <t>Table B1</t>
-  </si>
-  <si>
-    <t>Match 10</t>
-  </si>
-  <si>
-    <t>Match 12</t>
-  </si>
-  <si>
-    <t>Table B2</t>
-  </si>
-  <si>
     <t>TEAM 12002 SCHEDULE</t>
   </si>
   <si>
-    <t>Match 14</t>
+    <t>Match 9</t>
+  </si>
+  <si>
+    <t>Match 11</t>
+  </si>
+  <si>
+    <t>Match 13</t>
+  </si>
+  <si>
+    <t>Match 15</t>
   </si>
   <si>
     <t>TEAM 12003 SCHEDULE</t>
@@ -196,6 +208,9 @@
     <t>Match 1</t>
   </si>
   <si>
+    <t>Match 16</t>
+  </si>
+  <si>
     <t>TEAM 12004 SCHEDULE</t>
   </si>
   <si>
@@ -208,12 +223,6 @@
     <t>Match 5</t>
   </si>
   <si>
-    <t>Match 11</t>
-  </si>
-  <si>
-    <t>Match 13</t>
-  </si>
-  <si>
     <t>TEAM 12006 SCHEDULE</t>
   </si>
   <si>
@@ -226,13 +235,7 @@
     <t>Match 2</t>
   </si>
   <si>
-    <t>Match 15</t>
-  </si>
-  <si>
     <t>TEAM 12008 SCHEDULE</t>
-  </si>
-  <si>
-    <t>Match 9</t>
   </si>
   <si>
     <t>TEAM 12009 SCHEDULE</t>
@@ -632,7 +635,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -700,9 +703,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3">
-        <v>12009</v>
-      </c>
+      <c r="D4" s="3"/>
       <c r="E4" s="3">
         <v>12007</v>
       </c>
@@ -717,12 +718,14 @@
       <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3">
+        <v>12004</v>
+      </c>
       <c r="D5" s="3">
+        <v>12009</v>
+      </c>
+      <c r="E5" s="3">
         <v>12006</v>
-      </c>
-      <c r="E5" s="3">
-        <v>12004</v>
       </c>
       <c r="F5" s="3">
         <v>12005</v>
@@ -735,17 +738,13 @@
       <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3">
         <v>12001</v>
       </c>
-      <c r="D6" s="3">
+      <c r="F6" s="3">
         <v>12007</v>
-      </c>
-      <c r="E6" s="3">
-        <v>12008</v>
-      </c>
-      <c r="F6" s="3">
-        <v>12009</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -756,13 +755,17 @@
         <v>11</v>
       </c>
       <c r="C7" s="3">
+        <v>12005</v>
+      </c>
+      <c r="D7" s="3">
+        <v>12008</v>
+      </c>
+      <c r="E7" s="3">
         <v>12006</v>
       </c>
-      <c r="D7" s="3">
-        <v>12005</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3">
+        <v>12009</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="3">
@@ -771,17 +774,13 @@
       <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
         <v>12002</v>
       </c>
-      <c r="D8" s="3">
+      <c r="F8" s="3">
         <v>12001</v>
-      </c>
-      <c r="E8" s="3">
-        <v>12009</v>
-      </c>
-      <c r="F8" s="3">
-        <v>12007</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -791,13 +790,17 @@
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="3">
+        <v>12006</v>
+      </c>
+      <c r="D9" s="3">
+        <v>12007</v>
+      </c>
       <c r="E9" s="3">
-        <v>12006</v>
+        <v>12008</v>
       </c>
       <c r="F9" s="3">
-        <v>12008</v>
+        <v>12009</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -808,17 +811,13 @@
         <v>14</v>
       </c>
       <c r="C10" s="3">
-        <v>12007</v>
+        <v>12001</v>
       </c>
       <c r="D10" s="3">
-        <v>12002</v>
-      </c>
-      <c r="E10" s="3">
-        <v>12001</v>
-      </c>
-      <c r="F10" s="3">
         <v>12003</v>
       </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="3">
@@ -828,13 +827,17 @@
         <v>15</v>
       </c>
       <c r="C11" s="3">
+        <v>12007</v>
+      </c>
+      <c r="D11" s="3">
+        <v>12002</v>
+      </c>
+      <c r="E11" s="3">
         <v>12009</v>
       </c>
-      <c r="D11" s="3">
+      <c r="F11" s="3">
         <v>12008</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="3">
@@ -843,17 +846,13 @@
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3">
+        <v>12001</v>
+      </c>
+      <c r="F12" s="3">
         <v>12004</v>
-      </c>
-      <c r="D12" s="3">
-        <v>12001</v>
-      </c>
-      <c r="E12" s="3">
-        <v>12003</v>
-      </c>
-      <c r="F12" s="3">
-        <v>12002</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -864,14 +863,16 @@
         <v>17</v>
       </c>
       <c r="C13" s="3">
-        <v>12005</v>
+        <v>12002</v>
       </c>
       <c r="D13" s="3">
         <v>12008</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3">
+        <v>12003</v>
+      </c>
       <c r="F13" s="3">
-        <v>12009</v>
+        <v>12005</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -882,17 +883,13 @@
         <v>18</v>
       </c>
       <c r="C14" s="3">
-        <v>12004</v>
+        <v>12009</v>
       </c>
       <c r="D14" s="3">
-        <v>12003</v>
-      </c>
-      <c r="E14" s="3">
-        <v>12002</v>
-      </c>
-      <c r="F14" s="3">
         <v>12001</v>
       </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="3">
@@ -901,13 +898,17 @@
       <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="C15" s="3">
+        <v>12004</v>
+      </c>
+      <c r="D15" s="3">
+        <v>12006</v>
+      </c>
       <c r="E15" s="3">
-        <v>12005</v>
+        <v>12002</v>
       </c>
       <c r="F15" s="3">
-        <v>12006</v>
+        <v>12003</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -918,15 +919,9 @@
         <v>20</v>
       </c>
       <c r="C16" s="3"/>
-      <c r="D16" s="3">
-        <v>12003</v>
-      </c>
-      <c r="E16" s="3">
-        <v>12002</v>
-      </c>
-      <c r="F16" s="3">
-        <v>12004</v>
-      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="3">
@@ -935,11 +930,31 @@
       <c r="B17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="C17" s="3">
+        <v>12007</v>
+      </c>
+      <c r="D17" s="3">
+        <v>12005</v>
+      </c>
+      <c r="E17" s="3">
+        <v>12004</v>
+      </c>
       <c r="F17" s="3">
-        <v>12007</v>
+        <v>12002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3">
+        <v>12003</v>
       </c>
     </row>
   </sheetData>
@@ -963,7 +978,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -973,10 +988,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -984,21 +999,21 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1006,43 +1021,43 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1066,7 +1081,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1076,10 +1091,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1087,10 +1102,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1098,21 +1113,21 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1120,32 +1135,32 @@
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1169,7 +1184,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1179,10 +1194,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1190,10 +1205,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1201,10 +1216,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1212,21 +1227,21 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1234,21 +1249,21 @@
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1272,7 +1287,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1282,10 +1297,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1293,10 +1308,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1304,10 +1319,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1315,10 +1330,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1326,21 +1341,21 @@
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1348,10 +1363,10 @@
         <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1375,7 +1390,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1385,10 +1400,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1396,10 +1411,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1407,43 +1422,43 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1451,10 +1466,10 @@
         <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1478,7 +1493,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1488,10 +1503,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1499,21 +1514,21 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1521,10 +1536,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1532,10 +1547,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1543,21 +1558,21 @@
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1581,7 +1596,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1591,43 +1606,43 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1635,32 +1650,32 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1685,7 +1700,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1" s="4"/>
     </row>
@@ -1694,12 +1709,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3">
         <v>12001</v>
@@ -1707,7 +1722,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3">
         <v>12002</v>
@@ -1715,7 +1730,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3">
         <v>12003</v>
@@ -1723,7 +1738,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3">
         <v>12004</v>
@@ -1731,7 +1746,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="3">
         <v>12005</v>
@@ -1739,7 +1754,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3">
         <v>12006</v>
@@ -1747,7 +1762,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3">
         <v>12007</v>
@@ -1755,7 +1770,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" s="3">
         <v>12008</v>
@@ -1763,7 +1778,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3">
         <v>12009</v>
@@ -1779,7 +1794,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1790,7 +1805,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -1799,7 +1814,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1812,10 +1827,10 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>12001</v>
+        <v>12004</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1823,15 +1838,15 @@
         <v>11</v>
       </c>
       <c r="B5" s="3">
-        <v>12006</v>
+        <v>12005</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" s="3">
-        <v>12002</v>
+        <v>12006</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1839,7 +1854,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="3">
-        <v>12007</v>
+        <v>12001</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1847,31 +1862,39 @@
         <v>15</v>
       </c>
       <c r="B8" s="3">
-        <v>12009</v>
+        <v>12007</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3">
-        <v>12004</v>
+        <v>12002</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3">
-        <v>12005</v>
+        <v>12009</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3">
         <v>12004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3">
+        <v>12007</v>
       </c>
     </row>
   </sheetData>
@@ -1883,6 +1906,119 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3">
+        <v>12004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3">
+        <v>12007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3">
+        <v>12003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="3">
+        <v>12002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3">
+        <v>12005</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -1895,7 +2031,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -1904,7 +2040,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1912,7 +2048,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="3">
-        <v>12004</v>
+        <v>12005</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1920,7 +2056,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="3">
-        <v>12009</v>
+        <v>12007</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1936,7 +2072,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="3">
-        <v>12007</v>
+        <v>12001</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1944,7 +2080,7 @@
         <v>11</v>
       </c>
       <c r="B7" s="3">
-        <v>12005</v>
+        <v>12006</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1952,15 +2088,15 @@
         <v>12</v>
       </c>
       <c r="B8" s="3">
-        <v>12001</v>
+        <v>12002</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3">
-        <v>12002</v>
+        <v>12008</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1968,7 +2104,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>12008</v>
+        <v>12009</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1984,144 +2120,23 @@
         <v>17</v>
       </c>
       <c r="B12" s="3">
-        <v>12008</v>
+        <v>12003</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" s="3">
-        <v>12003</v>
+        <v>12002</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3">
-        <v>12003</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3">
-        <v>12005</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="3">
-        <v>12007</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3">
         <v>12004</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="3">
-        <v>12008</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="3">
-        <v>12009</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="3">
-        <v>12006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="3">
-        <v>12001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="3">
-        <v>12003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="3">
-        <v>12002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="3">
-        <v>12005</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="3">
-        <v>12002</v>
       </c>
     </row>
   </sheetData>
@@ -2145,7 +2160,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -2154,7 +2169,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2186,55 +2201,55 @@
         <v>10</v>
       </c>
       <c r="B6" s="3">
-        <v>12009</v>
+        <v>12007</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B7" s="3">
-        <v>12007</v>
+        <v>12009</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3">
-        <v>12008</v>
+        <v>12001</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="3">
-        <v>12003</v>
+        <v>12009</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="3">
-        <v>12002</v>
+        <v>12008</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="3">
-        <v>12009</v>
+        <v>12004</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12" s="3">
-        <v>12001</v>
+        <v>12005</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2242,23 +2257,23 @@
         <v>19</v>
       </c>
       <c r="B13" s="3">
-        <v>12006</v>
+        <v>12003</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" s="3">
-        <v>12004</v>
+        <v>12002</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B15" s="3">
-        <v>12007</v>
+        <v>12003</v>
       </c>
     </row>
   </sheetData>
@@ -2285,7 +2300,7 @@
         <v>4</v>
       </c>
       <c r="C1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2296,7 +2311,7 @@
         <v>6</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2307,7 +2322,7 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2318,7 +2333,7 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2329,7 +2344,7 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2340,7 +2355,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2348,7 +2363,7 @@
         <v>12002</v>
       </c>
       <c r="B7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -2359,10 +2374,10 @@
         <v>12002</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2370,7 +2385,7 @@
         <v>12002</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -2381,10 +2396,10 @@
         <v>12002</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2406,7 +2421,7 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2414,7 +2429,7 @@
         <v>12003</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -2425,10 +2440,10 @@
         <v>12003</v>
       </c>
       <c r="B14">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2436,10 +2451,10 @@
         <v>12003</v>
       </c>
       <c r="B15">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C15">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2461,7 +2476,7 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2472,7 +2487,7 @@
         <v>10</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2480,7 +2495,7 @@
         <v>12004</v>
       </c>
       <c r="B19">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2491,10 +2506,10 @@
         <v>12004</v>
       </c>
       <c r="B20">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2527,7 +2542,7 @@
         <v>5</v>
       </c>
       <c r="C23">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2538,7 +2553,7 @@
         <v>11</v>
       </c>
       <c r="C24">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2546,10 +2561,10 @@
         <v>12005</v>
       </c>
       <c r="B25">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C25">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2571,7 +2586,7 @@
         <v>3</v>
       </c>
       <c r="C27">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2582,7 +2597,7 @@
         <v>5</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2593,7 +2608,7 @@
         <v>7</v>
       </c>
       <c r="C29">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2604,7 +2619,7 @@
         <v>13</v>
       </c>
       <c r="C30">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2626,7 +2641,7 @@
         <v>4</v>
       </c>
       <c r="C32">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2634,10 +2649,10 @@
         <v>12007</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C33">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2645,7 +2660,7 @@
         <v>12007</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -2659,7 +2674,7 @@
         <v>15</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2678,10 +2693,10 @@
         <v>12008</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C37">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2692,7 +2707,7 @@
         <v>7</v>
       </c>
       <c r="C38">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2703,7 +2718,7 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2722,7 +2737,7 @@
         <v>12009</v>
       </c>
       <c r="B41">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -2733,7 +2748,7 @@
         <v>12009</v>
       </c>
       <c r="B42">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>4</v>
@@ -2744,10 +2759,10 @@
         <v>12009</v>
       </c>
       <c r="B43">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2758,7 +2773,7 @@
         <v>9</v>
       </c>
       <c r="C44">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2766,10 +2781,10 @@
         <v>12009</v>
       </c>
       <c r="B45">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C45">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2790,7 +2805,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2800,21 +2815,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2822,10 +2837,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2833,10 +2848,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2844,10 +2859,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2855,10 +2870,10 @@
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2866,10 +2881,10 @@
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2893,7 +2908,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -2903,21 +2918,21 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2925,54 +2940,54 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add full page table printout
</commit_message>
<xml_diff>
--- a/scheduler/schedule.xlsx
+++ b/scheduler/schedule.xlsx
@@ -10,26 +10,30 @@
     <sheet name="Match Schedule" sheetId="1" r:id="rId1"/>
     <sheet name="Judging Schedule" sheetId="2" r:id="rId2"/>
     <sheet name="Table R1 Schedule" sheetId="3" r:id="rId3"/>
-    <sheet name="Table R2 Schedule" sheetId="4" r:id="rId4"/>
-    <sheet name="Table B1 Schedule" sheetId="5" r:id="rId5"/>
-    <sheet name="Table B2 Schedule" sheetId="6" r:id="rId6"/>
-    <sheet name="All Matches" sheetId="7" r:id="rId7"/>
-    <sheet name="Team 12001 Schedule" sheetId="8" r:id="rId8"/>
-    <sheet name="Team 12002 Schedule" sheetId="9" r:id="rId9"/>
-    <sheet name="Team 12003 Schedule" sheetId="10" r:id="rId10"/>
-    <sheet name="Team 12004 Schedule" sheetId="11" r:id="rId11"/>
-    <sheet name="Team 12005 Schedule" sheetId="12" r:id="rId12"/>
-    <sheet name="Team 12006 Schedule" sheetId="13" r:id="rId13"/>
-    <sheet name="Team 12007 Schedule" sheetId="14" r:id="rId14"/>
-    <sheet name="Team 12008 Schedule" sheetId="15" r:id="rId15"/>
-    <sheet name="Team 12009 Schedule" sheetId="16" r:id="rId16"/>
+    <sheet name="Table R1 Schedule (full)" sheetId="4" r:id="rId4"/>
+    <sheet name="Table R2 Schedule" sheetId="5" r:id="rId5"/>
+    <sheet name="Table R2 Schedule (full)" sheetId="6" r:id="rId6"/>
+    <sheet name="Table B1 Schedule" sheetId="7" r:id="rId7"/>
+    <sheet name="Table B1 Schedule (full)" sheetId="8" r:id="rId8"/>
+    <sheet name="Table B2 Schedule" sheetId="9" r:id="rId9"/>
+    <sheet name="Table B2 Schedule (full)" sheetId="10" r:id="rId10"/>
+    <sheet name="All Matches" sheetId="11" r:id="rId11"/>
+    <sheet name="Team 12001 Schedule" sheetId="12" r:id="rId12"/>
+    <sheet name="Team 12002 Schedule" sheetId="13" r:id="rId13"/>
+    <sheet name="Team 12003 Schedule" sheetId="14" r:id="rId14"/>
+    <sheet name="Team 12004 Schedule" sheetId="15" r:id="rId15"/>
+    <sheet name="Team 12005 Schedule" sheetId="16" r:id="rId16"/>
+    <sheet name="Team 12006 Schedule" sheetId="17" r:id="rId17"/>
+    <sheet name="Team 12007 Schedule" sheetId="18" r:id="rId18"/>
+    <sheet name="Team 12008 Schedule" sheetId="19" r:id="rId19"/>
+    <sheet name="Team 12009 Schedule" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="69">
   <si>
     <t>OFFICIAL ROBOT ROUNDS SCHEDULE</t>
   </si>
@@ -242,7 +246,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -253,6 +257,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="30"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -280,7 +307,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFC266"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -337,6 +364,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -952,102 +988,136 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+    <col min="1" max="2" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2" ht="35" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+    </row>
+    <row r="2" spans="1:2" ht="35" customHeight="1">
+      <c r="A2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="35" customHeight="1">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
+      <c r="B3" s="9">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="35" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="35" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9">
+        <v>12005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="35" customHeight="1">
+      <c r="A6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="35" customHeight="1">
+      <c r="A7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9">
+        <v>12007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="35" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="9">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="35" customHeight="1">
+      <c r="A9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
+      <c r="B9" s="9">
+        <v>12003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="35" customHeight="1">
+      <c r="A10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
+      <c r="B10" s="9">
+        <v>12002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="35" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="9">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="35" customHeight="1">
+      <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
+      <c r="B12" s="9">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="35" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="9">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="35" customHeight="1">
+      <c r="A14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>45</v>
+      <c r="B14" s="9">
+        <v>12004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="35" customHeight="1">
+      <c r="A15" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="9">
+        <v>12007</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1055,103 +1125,508 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="18.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="A1">
+        <v>12001</v>
+      </c>
+      <c r="B1">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2">
+        <v>12001</v>
+      </c>
+      <c r="B2">
+        <v>6</v>
+      </c>
+      <c r="C2">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
+      <c r="A3">
+        <v>12001</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>12001</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>12001</v>
+      </c>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>12002</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>12002</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>12002</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>12002</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>12002</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>12003</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>12003</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12003</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>12003</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>12003</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>12004</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>12004</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>12004</v>
+      </c>
+      <c r="B18">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>12004</v>
+      </c>
+      <c r="B19">
+        <v>12</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>12004</v>
+      </c>
+      <c r="B20">
+        <v>14</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>12005</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>12005</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>12005</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>12005</v>
+      </c>
+      <c r="B24">
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>12005</v>
+      </c>
+      <c r="B25">
+        <v>13</v>
+      </c>
+      <c r="C25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>12006</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>12006</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>12006</v>
+      </c>
+      <c r="B28">
+        <v>5</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>12006</v>
+      </c>
+      <c r="B29">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
+      <c r="C29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>12006</v>
+      </c>
+      <c r="B30">
+        <v>13</v>
+      </c>
+      <c r="C30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>12007</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>12007</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>12007</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>12007</v>
+      </c>
+      <c r="B34">
+        <v>8</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>12007</v>
+      </c>
+      <c r="B35">
+        <v>15</v>
+      </c>
+      <c r="C35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>12008</v>
+      </c>
+      <c r="B36">
+        <v>2</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>12008</v>
+      </c>
+      <c r="B37">
+        <v>4</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>12008</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+      <c r="C38">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>12008</v>
+      </c>
+      <c r="B39">
         <v>9</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>50</v>
+      <c r="C39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>12008</v>
+      </c>
+      <c r="B40">
+        <v>11</v>
+      </c>
+      <c r="C40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>12009</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>12009</v>
+      </c>
+      <c r="B42">
+        <v>4</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>12009</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
+      </c>
+      <c r="C43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44">
+        <v>12009</v>
+      </c>
+      <c r="B44">
+        <v>9</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>12009</v>
+      </c>
+      <c r="B45">
+        <v>11</v>
+      </c>
+      <c r="C45">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1168,11 +1643,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="A1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
@@ -1187,32 +1662,32 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>45</v>
@@ -1220,35 +1695,35 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1271,11 +1746,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="A1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
@@ -1290,68 +1765,68 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1374,11 +1849,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="A1" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
@@ -1393,32 +1868,32 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>50</v>
@@ -1426,35 +1901,35 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1477,11 +1952,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="A1" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
@@ -1496,21 +1971,21 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>47</v>
@@ -1518,46 +1993,46 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="3" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>23</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1580,11 +2055,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
+      <c r="A1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
@@ -1599,13 +2074,219 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1616,7 +2297,7 @@
         <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1627,7 +2308,110 @@
         <v>44</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1638,7 +2422,7 @@
         <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1649,12 +2433,12 @@
         <v>59</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>41</v>
@@ -1777,6 +2561,109 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="3" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B11"/>
@@ -1884,6 +2771,111 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="35" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" ht="35" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="35" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9">
+        <v>12003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="35" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="9">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="35" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="9">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="35" customHeight="1">
+      <c r="A6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="9">
+        <v>12002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="35" customHeight="1">
+      <c r="A7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9">
+        <v>12007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="35" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="9">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="35" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="9">
+        <v>12004</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="35" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="9">
+        <v>12005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="35" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="9">
+        <v>12004</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2011,7 +3003,136 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="35" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" ht="35" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="35" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9">
+        <v>12004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="35" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="35" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="35" customHeight="1">
+      <c r="A6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
+        <v>12007</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="35" customHeight="1">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9">
+        <v>12005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="35" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="9">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="35" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="9">
+        <v>12002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="35" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="35" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="9">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="35" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="9">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="35" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="9">
+        <v>12003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="35" customHeight="1">
+      <c r="A14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="9">
+        <v>12003</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -2132,7 +3253,128 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="35" customHeight="1">
+      <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="7"/>
+    </row>
+    <row r="2" spans="1:2" ht="35" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="35" customHeight="1">
+      <c r="A3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="9">
+        <v>12005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="35" customHeight="1">
+      <c r="A4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="9">
+        <v>12007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="35" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="9">
+        <v>12004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="35" customHeight="1">
+      <c r="A6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
+        <v>12008</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="35" customHeight="1">
+      <c r="A7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="9">
+        <v>12009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="35" customHeight="1">
+      <c r="A8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="9">
+        <v>12006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="35" customHeight="1">
+      <c r="A9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="9">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="35" customHeight="1">
+      <c r="A10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="9">
+        <v>12003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="35" customHeight="1">
+      <c r="A11" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="9">
+        <v>12002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="35" customHeight="1">
+      <c r="A12" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="9">
+        <v>12005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="35" customHeight="1">
+      <c r="A13" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="9">
+        <v>12002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -2267,718 +3509,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C45"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1">
-        <v>12001</v>
-      </c>
-      <c r="B1">
-        <v>4</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>12001</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>12001</v>
-      </c>
-      <c r="B3">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>12001</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>12001</v>
-      </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6">
-        <v>12002</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7">
-        <v>12002</v>
-      </c>
-      <c r="B7">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8">
-        <v>12002</v>
-      </c>
-      <c r="B8">
-        <v>10</v>
-      </c>
-      <c r="C8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9">
-        <v>12002</v>
-      </c>
-      <c r="B9">
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10">
-        <v>12002</v>
-      </c>
-      <c r="B10">
-        <v>14</v>
-      </c>
-      <c r="C10">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11">
-        <v>12003</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12">
-        <v>12003</v>
-      </c>
-      <c r="B12">
-        <v>8</v>
-      </c>
-      <c r="C12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13">
-        <v>12003</v>
-      </c>
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14">
-        <v>12003</v>
-      </c>
-      <c r="B14">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15">
-        <v>12003</v>
-      </c>
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16">
-        <v>12004</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17">
-        <v>12004</v>
-      </c>
-      <c r="B17">
-        <v>3</v>
-      </c>
-      <c r="C17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18">
-        <v>12004</v>
-      </c>
-      <c r="B18">
-        <v>10</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19">
-        <v>12004</v>
-      </c>
-      <c r="B19">
-        <v>12</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20">
-        <v>12004</v>
-      </c>
-      <c r="B20">
-        <v>14</v>
-      </c>
-      <c r="C20">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21">
-        <v>12005</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22">
-        <v>12005</v>
-      </c>
-      <c r="B22">
-        <v>3</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23">
-        <v>12005</v>
-      </c>
-      <c r="B23">
-        <v>5</v>
-      </c>
-      <c r="C23">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24">
-        <v>12005</v>
-      </c>
-      <c r="B24">
-        <v>11</v>
-      </c>
-      <c r="C24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25">
-        <v>12005</v>
-      </c>
-      <c r="B25">
-        <v>13</v>
-      </c>
-      <c r="C25">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26">
-        <v>12006</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27">
-        <v>12006</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28">
-        <v>12006</v>
-      </c>
-      <c r="B28">
-        <v>5</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29">
-        <v>12006</v>
-      </c>
-      <c r="B29">
-        <v>7</v>
-      </c>
-      <c r="C29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30">
-        <v>12006</v>
-      </c>
-      <c r="B30">
-        <v>13</v>
-      </c>
-      <c r="C30">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31">
-        <v>12007</v>
-      </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32">
-        <v>12007</v>
-      </c>
-      <c r="B32">
-        <v>4</v>
-      </c>
-      <c r="C32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33">
-        <v>12007</v>
-      </c>
-      <c r="B33">
-        <v>6</v>
-      </c>
-      <c r="C33">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34">
-        <v>12007</v>
-      </c>
-      <c r="B34">
-        <v>8</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35">
-        <v>12007</v>
-      </c>
-      <c r="B35">
-        <v>15</v>
-      </c>
-      <c r="C35">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36">
-        <v>12008</v>
-      </c>
-      <c r="B36">
-        <v>2</v>
-      </c>
-      <c r="C36">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37">
-        <v>12008</v>
-      </c>
-      <c r="B37">
-        <v>4</v>
-      </c>
-      <c r="C37">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38">
-        <v>12008</v>
-      </c>
-      <c r="B38">
-        <v>7</v>
-      </c>
-      <c r="C38">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39">
-        <v>12008</v>
-      </c>
-      <c r="B39">
-        <v>9</v>
-      </c>
-      <c r="C39">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40">
-        <v>12008</v>
-      </c>
-      <c r="B40">
-        <v>11</v>
-      </c>
-      <c r="C40">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41">
-        <v>12009</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="C41">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42">
-        <v>12009</v>
-      </c>
-      <c r="B42">
-        <v>4</v>
-      </c>
-      <c r="C42">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43">
-        <v>12009</v>
-      </c>
-      <c r="B43">
-        <v>6</v>
-      </c>
-      <c r="C43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44">
-        <v>12009</v>
-      </c>
-      <c r="B44">
-        <v>9</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45">
-        <v>12009</v>
-      </c>
-      <c r="B45">
-        <v>11</v>
-      </c>
-      <c r="C45">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="18.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="3" width="18.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add match number to table sheets
</commit_message>
<xml_diff>
--- a/scheduler/schedule.xlsx
+++ b/scheduler/schedule.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="70">
   <si>
     <t>OFFICIAL ROBOT ROUNDS SCHEDULE</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>TABLE R1 SCHEDULE</t>
+  </si>
+  <si>
+    <t>Match</t>
   </si>
   <si>
     <t>Team</t>
@@ -988,137 +991,181 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="40.7109375" customWidth="1"/>
+    <col min="1" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="35" customHeight="1">
+    <row r="1" spans="1:3" ht="35" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:2" ht="35" customHeight="1">
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" ht="35" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="35" customHeight="1">
-      <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="35" customHeight="1">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9">
+      <c r="C3" s="9">
         <v>12006</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="35" customHeight="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:3" ht="35" customHeight="1">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9">
+      <c r="C4" s="9">
         <v>12008</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="35" customHeight="1">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:3" ht="35" customHeight="1">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9">
+      <c r="C5" s="9">
         <v>12005</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="35" customHeight="1">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:3" ht="35" customHeight="1">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="9">
+      <c r="C6" s="9">
         <v>12009</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="35" customHeight="1">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:3" ht="35" customHeight="1">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9">
+      <c r="C7" s="9">
         <v>12007</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="35" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:3" ht="35" customHeight="1">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="9">
+      <c r="C8" s="9">
         <v>12008</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="35" customHeight="1">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:3" ht="35" customHeight="1">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="9">
+      <c r="C9" s="9">
         <v>12003</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="35" customHeight="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:3" ht="35" customHeight="1">
+      <c r="A10" s="9">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="9">
+      <c r="C10" s="9">
         <v>12002</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="35" customHeight="1">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:3" ht="35" customHeight="1">
+      <c r="A11" s="9">
+        <v>11</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="9">
+      <c r="C11" s="9">
         <v>12009</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="35" customHeight="1">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:3" ht="35" customHeight="1">
+      <c r="A12" s="9">
+        <v>12</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="9">
+      <c r="C12" s="9">
         <v>12001</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="35" customHeight="1">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:3" ht="35" customHeight="1">
+      <c r="A13" s="9">
+        <v>13</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="9">
+      <c r="C13" s="9">
         <v>12006</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="35" customHeight="1">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:3" ht="35" customHeight="1">
+      <c r="A14" s="9">
+        <v>14</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="9">
+      <c r="C14" s="9">
         <v>12004</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="35" customHeight="1">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:3" ht="35" customHeight="1">
+      <c r="A15" s="9">
+        <v>15</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="9">
+      <c r="C15" s="9">
         <v>12007</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1644,7 +1691,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1654,10 +1701,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1665,7 +1712,7 @@
         <v>24</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>23</v>
@@ -1676,10 +1723,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1687,10 +1734,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1698,10 +1745,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1709,10 +1756,10 @@
         <v>16</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1720,10 +1767,10 @@
         <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1747,7 +1794,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1757,10 +1804,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1768,7 +1815,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>23</v>
@@ -1779,10 +1826,10 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1790,10 +1837,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1801,10 +1848,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1812,10 +1859,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1823,10 +1870,10 @@
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1850,7 +1897,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1860,10 +1907,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1871,10 +1918,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1882,7 +1929,7 @@
         <v>26</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>23</v>
@@ -1893,10 +1940,10 @@
         <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1904,10 +1951,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1915,10 +1962,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1926,10 +1973,10 @@
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1953,7 +2000,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1963,10 +2010,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1974,10 +2021,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1985,10 +2032,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1996,7 +2043,7 @@
         <v>27</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>23</v>
@@ -2007,10 +2054,10 @@
         <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2018,10 +2065,10 @@
         <v>18</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2029,10 +2076,10 @@
         <v>20</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2056,7 +2103,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2066,10 +2113,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2077,10 +2124,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2088,10 +2135,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2099,10 +2146,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2110,7 +2157,7 @@
         <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>23</v>
@@ -2121,10 +2168,10 @@
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2132,10 +2179,10 @@
         <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2159,7 +2206,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2169,10 +2216,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2180,10 +2227,10 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2191,10 +2238,10 @@
         <v>9</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2202,10 +2249,10 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2213,10 +2260,10 @@
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2224,7 +2271,7 @@
         <v>29</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>23</v>
@@ -2235,10 +2282,10 @@
         <v>19</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2262,7 +2309,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2272,10 +2319,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2283,10 +2330,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2294,10 +2341,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2305,10 +2352,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2316,10 +2363,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2327,7 +2374,7 @@
         <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>23</v>
@@ -2338,10 +2385,10 @@
         <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2365,7 +2412,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2375,10 +2422,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2386,10 +2433,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2397,10 +2444,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2408,10 +2455,10 @@
         <v>13</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2419,10 +2466,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2430,10 +2477,10 @@
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2441,7 +2488,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>23</v>
@@ -2574,7 +2621,7 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2584,10 +2631,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -2595,10 +2642,10 @@
         <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2606,10 +2653,10 @@
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2617,10 +2664,10 @@
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2628,10 +2675,10 @@
         <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2639,10 +2686,10 @@
         <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2650,7 +2697,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>23</v>
@@ -2666,104 +2713,135 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3">
+      <c r="C3" s="3">
         <v>12003</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="3">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>12001</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="3">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="3">
+      <c r="C5" s="3">
         <v>12006</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="3">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="3">
+      <c r="C6" s="3">
         <v>12002</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="3">
+        <v>8</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="3">
         <v>12007</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3">
+      <c r="C8" s="3">
         <v>12009</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>10</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3">
+      <c r="C9" s="3">
         <v>12004</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
+        <v>11</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3">
+      <c r="C10" s="3">
         <v>12005</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="3">
+      <c r="C11" s="3">
         <v>12004</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2771,233 +2849,305 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="40.7109375" customWidth="1"/>
+    <col min="1" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="35" customHeight="1">
+    <row r="1" spans="1:3" ht="35" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>33</v>
       </c>
       <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:2" ht="35" customHeight="1">
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" ht="35" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="35" customHeight="1">
-      <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="35" customHeight="1">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9">
+      <c r="C3" s="9">
         <v>12003</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="35" customHeight="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:3" ht="35" customHeight="1">
+      <c r="A4" s="9">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9">
+      <c r="C4" s="9">
         <v>12001</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="35" customHeight="1">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:3" ht="35" customHeight="1">
+      <c r="A5" s="9">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="9">
+      <c r="C5" s="9">
         <v>12006</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="35" customHeight="1">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:3" ht="35" customHeight="1">
+      <c r="A6" s="9">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="9">
+      <c r="C6" s="9">
         <v>12002</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="35" customHeight="1">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:3" ht="35" customHeight="1">
+      <c r="A7" s="9">
+        <v>8</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="9">
+      <c r="C7" s="9">
         <v>12007</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="35" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:3" ht="35" customHeight="1">
+      <c r="A8" s="9">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="9">
+      <c r="C8" s="9">
         <v>12009</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="35" customHeight="1">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:3" ht="35" customHeight="1">
+      <c r="A9" s="9">
+        <v>10</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="9">
+      <c r="C9" s="9">
         <v>12004</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="35" customHeight="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:3" ht="35" customHeight="1">
+      <c r="A10" s="9">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="9">
+      <c r="C10" s="9">
         <v>12005</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="35" customHeight="1">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:3" ht="35" customHeight="1">
+      <c r="A11" s="9">
+        <v>12</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="9">
+      <c r="C11" s="9">
         <v>12004</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3">
+      <c r="C3" s="3">
         <v>12004</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>12009</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3">
+      <c r="C5" s="3">
         <v>12006</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3">
+      <c r="C6" s="3">
         <v>12007</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="3">
         <v>12005</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3">
+      <c r="C8" s="3">
         <v>12001</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3">
+      <c r="C9" s="3">
         <v>12002</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3">
+      <c r="C10" s="3">
         <v>12008</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3">
+      <c r="C11" s="3">
         <v>12001</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3">
+      <c r="C12" s="3">
         <v>12008</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3">
+      <c r="C13" s="3">
         <v>12003</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="3">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="3">
+      <c r="C14" s="3">
         <v>12003</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3005,249 +3155,327 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="40.7109375" customWidth="1"/>
+    <col min="1" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="35" customHeight="1">
+    <row r="1" spans="1:3" ht="35" customHeight="1">
       <c r="A1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" ht="35" customHeight="1">
+      <c r="A2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:2" ht="35" customHeight="1">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="35" customHeight="1">
-      <c r="A3" s="9" t="s">
+    </row>
+    <row r="3" spans="1:3" ht="35" customHeight="1">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9">
+      <c r="C3" s="9">
         <v>12004</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="35" customHeight="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:3" ht="35" customHeight="1">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9">
+      <c r="C4" s="9">
         <v>12009</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="35" customHeight="1">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:3" ht="35" customHeight="1">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9">
+      <c r="C5" s="9">
         <v>12006</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="35" customHeight="1">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:3" ht="35" customHeight="1">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="9">
+      <c r="C6" s="9">
         <v>12007</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="35" customHeight="1">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:3" ht="35" customHeight="1">
+      <c r="A7" s="9">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="9">
+      <c r="C7" s="9">
         <v>12005</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="35" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:3" ht="35" customHeight="1">
+      <c r="A8" s="9">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="9">
+      <c r="C8" s="9">
         <v>12001</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="35" customHeight="1">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:3" ht="35" customHeight="1">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="9">
+      <c r="C9" s="9">
         <v>12002</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="35" customHeight="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:3" ht="35" customHeight="1">
+      <c r="A10" s="9">
+        <v>9</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="9">
+      <c r="C10" s="9">
         <v>12008</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="35" customHeight="1">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:3" ht="35" customHeight="1">
+      <c r="A11" s="9">
+        <v>10</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="9">
+      <c r="C11" s="9">
         <v>12001</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="35" customHeight="1">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:3" ht="35" customHeight="1">
+      <c r="A12" s="9">
+        <v>11</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="9">
+      <c r="C12" s="9">
         <v>12008</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="35" customHeight="1">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:3" ht="35" customHeight="1">
+      <c r="A13" s="9">
+        <v>12</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="9">
+      <c r="C13" s="9">
         <v>12003</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="35" customHeight="1">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:3" ht="35" customHeight="1">
+      <c r="A14" s="9">
+        <v>14</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="9">
+      <c r="C14" s="9">
         <v>12003</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3">
+      <c r="C3" s="3">
         <v>12005</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>12007</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3">
+      <c r="C5" s="3">
         <v>12004</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3">
+      <c r="C6" s="3">
         <v>12008</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="3">
         <v>12009</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3">
+      <c r="C8" s="3">
         <v>12006</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3">
+      <c r="C9" s="3">
         <v>12001</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3">
+      <c r="C10" s="3">
         <v>12003</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>12</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="3">
+      <c r="C11" s="3">
         <v>12002</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" s="3">
+        <v>13</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="3">
+      <c r="C12" s="3">
         <v>12005</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="3">
+      <c r="C13" s="3">
         <v>12002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3255,257 +3483,338 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="40.7109375" customWidth="1"/>
+    <col min="1" max="3" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="35" customHeight="1">
+    <row r="1" spans="1:3" ht="35" customHeight="1">
       <c r="A1" s="7" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="7"/>
-    </row>
-    <row r="2" spans="1:2" ht="35" customHeight="1">
+      <c r="C1" s="7"/>
+    </row>
+    <row r="2" spans="1:3" ht="35" customHeight="1">
       <c r="A2" s="8" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="35" customHeight="1">
-      <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="35" customHeight="1">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9">
+      <c r="C3" s="9">
         <v>12005</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="35" customHeight="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:3" ht="35" customHeight="1">
+      <c r="A4" s="9">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="9">
+      <c r="C4" s="9">
         <v>12007</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="35" customHeight="1">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:3" ht="35" customHeight="1">
+      <c r="A5" s="9">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9">
+      <c r="C5" s="9">
         <v>12004</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="35" customHeight="1">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:3" ht="35" customHeight="1">
+      <c r="A6" s="9">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="9">
+      <c r="C6" s="9">
         <v>12008</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="35" customHeight="1">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:3" ht="35" customHeight="1">
+      <c r="A7" s="9">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9">
+      <c r="C7" s="9">
         <v>12009</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="35" customHeight="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:3" ht="35" customHeight="1">
+      <c r="A8" s="9">
+        <v>7</v>
+      </c>
+      <c r="B8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="9">
+      <c r="C8" s="9">
         <v>12006</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="35" customHeight="1">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:3" ht="35" customHeight="1">
+      <c r="A9" s="9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="9">
+      <c r="C9" s="9">
         <v>12001</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="35" customHeight="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:3" ht="35" customHeight="1">
+      <c r="A10" s="9">
+        <v>10</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="9">
+      <c r="C10" s="9">
         <v>12003</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="35" customHeight="1">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:3" ht="35" customHeight="1">
+      <c r="A11" s="9">
+        <v>12</v>
+      </c>
+      <c r="B11" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="9">
+      <c r="C11" s="9">
         <v>12002</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="35" customHeight="1">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:3" ht="35" customHeight="1">
+      <c r="A12" s="9">
+        <v>13</v>
+      </c>
+      <c r="B12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="9">
+      <c r="C12" s="9">
         <v>12005</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="35" customHeight="1">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:3" ht="35" customHeight="1">
+      <c r="A13" s="9">
+        <v>14</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="9">
+      <c r="C13" s="9">
         <v>12002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
+  <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3">
+      <c r="C3" s="3">
         <v>12006</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="3">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>12008</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:3">
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3">
+      <c r="C5" s="3">
         <v>12005</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:3">
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3">
+      <c r="C6" s="3">
         <v>12009</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3">
+      <c r="C7" s="3">
         <v>12007</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3">
+      <c r="C8" s="3">
         <v>12008</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3">
+      <c r="C9" s="3">
         <v>12003</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
+        <v>10</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="3">
+      <c r="C10" s="3">
         <v>12002</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" s="3">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3">
+      <c r="C11" s="3">
         <v>12009</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3">
+      <c r="A12" s="3">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="3">
+      <c r="C12" s="3">
         <v>12001</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="3">
+      <c r="C13" s="3">
         <v>12006</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:3">
+      <c r="A14" s="3">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="3">
+      <c r="C14" s="3">
         <v>12004</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:3">
+      <c r="A15" s="3">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="3">
+      <c r="C15" s="3">
         <v>12007</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>